<commit_message>
Updated Security for Mini api flow
</commit_message>
<xml_diff>
--- a/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet_empty.xlsx
+++ b/samples/idaithalam-excel-apitesting/src/test/resources/virtualan_collection_pet_empty.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>ContentType</t>
+  </si>
+  <si>
+    <t>RequestHeaders</t>
   </si>
   <si>
     <t>RequestFile</t>
@@ -121,12 +124,40 @@
   <si>
     <t>Id=[petId];petName=doggie</t>
   </si>
+  <si>
+    <t>PetGet-Test</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Inconsolata,Arial"/>
+        <b/>
+        <color rgb="FF1155CC"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>https://live.virtualandemo.com/api/pets/findByTags?tags=</t>
+    </r>
+    <r>
+      <rPr>
+        <rFont val="Inconsolata,Arial"/>
+        <b/>
+        <color rgb="FF000000"/>
+        <sz val="11.0"/>
+        <u/>
+      </rPr>
+      <t>[tag]</t>
+    </r>
+  </si>
+  <si>
+    <t>test=Bearer [tag]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -149,8 +180,18 @@
       <color rgb="FF1155CC"/>
       <name val="Inconsolata"/>
     </font>
+    <font>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11.0"/>
+      <color rgb="FF1155CC"/>
+      <name val="Inconsolata"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +204,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7E1CD"/>
+        <bgColor rgb="FFB7E1CD"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -170,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -185,6 +232,24 @@
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,10 +480,10 @@
   <cols>
     <col customWidth="1" min="2" max="2" width="18.14"/>
     <col customWidth="1" min="3" max="3" width="176.14"/>
-    <col customWidth="1" min="6" max="6" width="24.71"/>
-    <col customWidth="1" min="7" max="7" width="23.29"/>
-    <col customWidth="1" min="11" max="11" width="49.29"/>
-    <col customWidth="1" min="12" max="12" width="24.29"/>
+    <col customWidth="1" min="7" max="7" width="24.71"/>
+    <col customWidth="1" min="8" max="8" width="23.29"/>
+    <col customWidth="1" min="12" max="12" width="49.29"/>
+    <col customWidth="1" min="13" max="13" width="24.29"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -434,7 +499,7 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -443,13 +508,13 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -458,87 +523,143 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>14</v>
+      <c r="A2" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="1">
+      <c r="I2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="3">
         <v>200.0</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="1">
+      <c r="I3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K3" s="1">
         <v>200.0</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="8"/>
+      <c r="K4" s="10">
+        <v>200.0</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="8" t="s">
         <v>22</v>
       </c>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2">
+  <conditionalFormatting sqref="G2">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(F2))&gt;0</formula>
+      <formula>LEN(TRIM(G2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C2"/>
     <hyperlink r:id="rId2" ref="C3"/>
+    <hyperlink r:id="rId3" ref="C4"/>
   </hyperlinks>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>